<commit_message>
mediciones de les cuadripepes
</commit_message>
<xml_diff>
--- a/TP5/Mediciones.xlsx
+++ b/TP5/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\Desktop\TP3 ELECTRO\TP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FAF7BC-50FA-44E7-BE7B-64721509DE95}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4975F4-CD71-487A-8B2A-651CDF5FC87E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDA36349-2CEE-46F1-A8FD-45D31E04EF72}"/>
   </bookViews>
@@ -406,10 +406,10 @@
     <t xml:space="preserve">Cuadripolo "X" - Nro. De serie: xxxx </t>
   </si>
   <si>
-    <t>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 20 mA)</t>
-  </si>
-  <si>
-    <t>Cuadripolo "A" - Nro. De serie: 9602 (15 V - 20 mA)</t>
+    <t>Cuadripolo "A" - Nro. De serie: 9608 (15 V - 50 mA) (T)</t>
+  </si>
+  <si>
+    <t>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,46 +567,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -926,38 +929,38 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
-      <c r="H1" s="20" t="s">
+      <c r="A1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+      <c r="H1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
       <c r="L1" s="6"/>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="R1" s="10" t="s">
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="R1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -973,28 +976,28 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11" t="str">
+      <c r="H2" s="13" t="str">
         <f>$A$1</f>
-        <v>Cuadripolo "A" - Nro. De serie: 9602 (15 V - 20 mA)</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+        <v>Cuadripolo "A" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="11" t="str">
+      <c r="M2" s="13" t="str">
         <f>$A$1</f>
-        <v>Cuadripolo "A" - Nro. De serie: 9602 (15 V - 20 mA)</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="R2" s="11" t="str">
+        <v>Cuadripolo "A" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
+      </c>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="R2" s="13" t="str">
         <f>$A$1</f>
-        <v>Cuadripolo "A" - Nro. De serie: 9602 (15 V - 20 mA)</v>
-      </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
+        <v>Cuadripolo "A" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
+      </c>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1003,9 +1006,17 @@
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="D3" s="1">
+        <f>0.5*23</f>
+        <v>11.5</v>
+      </c>
+      <c r="E3" s="1">
+        <f>32*0.5</f>
+        <v>16</v>
+      </c>
       <c r="H3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1048,110 +1059,134 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>3.05</v>
+      </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="H4" s="8" t="e">
+      <c r="D4" s="1">
+        <f>33.5*0.5</f>
+        <v>16.75</v>
+      </c>
+      <c r="E4" s="1">
+        <f>0.5*23</f>
+        <v>11.5</v>
+      </c>
+      <c r="H4" s="8">
         <f>B6/D6*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" s="8" t="e">
+        <v>371.95121951219505</v>
+      </c>
+      <c r="I4" s="8">
         <f>B5/E5*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J4" s="8" t="e">
+        <v>310.29411764705878</v>
+      </c>
+      <c r="J4" s="8">
         <f>C6/D6*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" s="8" t="e">
+        <v>266.46341463414632</v>
+      </c>
+      <c r="K4" s="8">
         <f>C5/E5*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" s="8" t="e">
+        <v>448.5294117647058</v>
+      </c>
+      <c r="M4" s="8">
         <f>D4/B4/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N4" s="8" t="e">
+        <v>5.4918032786885245E-3</v>
+      </c>
+      <c r="N4" s="8">
         <f>D3/C3/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O4" s="8" t="e">
+        <v>3.7704918032786887E-3</v>
+      </c>
+      <c r="O4" s="8">
         <f>E4/B4/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="8" t="e">
+        <v>3.7704918032786887E-3</v>
+      </c>
+      <c r="P4" s="8">
         <f>E3/C3/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" s="8" t="e">
+        <v>5.2459016393442632E-3</v>
+      </c>
+      <c r="R4" s="8">
         <f>B6/C6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S4" s="8" t="e">
+        <v>1.3958810068649885</v>
+      </c>
+      <c r="S4" s="8">
         <f>-B4/E4*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T4" s="8" t="e">
+        <v>-265.21739130434781</v>
+      </c>
+      <c r="T4" s="8">
         <f>D6/C6/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U4" s="8" t="e">
+        <v>3.7528604118993139E-3</v>
+      </c>
+      <c r="U4" s="8">
         <f>-D4/E4</f>
-        <v>#DIV/0!</v>
+        <v>-1.4565217391304348</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1">
+        <f>2.11</f>
+        <v>2.11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.05</v>
+      </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <f>0.1*68</f>
+        <v>6.8000000000000007</v>
+      </c>
     </row>
     <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="C6" s="24">
+        <f>2.185</f>
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <f>82*0.1</f>
+        <v>8.2000000000000011</v>
+      </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="H8" s="13" t="s">
+      <c r="A8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="H8" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="M8" s="12" t="s">
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="M8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="R8" s="10" t="s">
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="R8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
     </row>
     <row r="9" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
@@ -1167,27 +1202,27 @@
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="11" t="str">
+      <c r="H9" s="13" t="str">
         <f>$A$8</f>
-        <v>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 20 mA)</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="M9" s="11" t="str">
+        <v>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="M9" s="13" t="str">
         <f>$A$8</f>
-        <v>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 20 mA)</v>
-      </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="R9" s="11" t="str">
+        <v>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
+      </c>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="R9" s="13" t="str">
         <f>$A$8</f>
-        <v>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 20 mA)</v>
-      </c>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
+        <v>Cuadripolo "B" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
+      </c>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
     </row>
     <row r="10" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1196,9 +1231,17 @@
       <c r="B10" s="9">
         <v>0</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="9">
+        <v>3.05</v>
+      </c>
+      <c r="D10" s="9">
+        <f>83*0.5</f>
+        <v>41.5</v>
+      </c>
+      <c r="E10" s="9">
+        <f>60*0.5</f>
+        <v>30</v>
+      </c>
       <c r="H10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1240,97 +1283,122 @@
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="9">
+        <v>3.05</v>
+      </c>
       <c r="C11" s="9">
         <v>0</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="9">
+        <f>72*0.5</f>
+        <v>36</v>
+      </c>
+      <c r="E11" s="9">
+        <f>60.5*0.5</f>
+        <v>30.25</v>
+      </c>
       <c r="H11" s="8" t="e">
-        <f>B13/D13*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="8" t="e">
+        <f>D13/#REF!*1000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I11" s="8">
         <f>B12/E12*1000</f>
-        <v>#DIV/0!</v>
+        <v>157.35384615384615</v>
       </c>
       <c r="J11" s="8" t="e">
-        <f>C13/D13*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="8" t="e">
+        <f>C13/#REF!*1000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K11" s="8">
         <f>C12/E12*1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="8" t="e">
+        <v>187.69230769230768</v>
+      </c>
+      <c r="M11" s="8">
         <f>D11/B11/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="8" t="e">
+        <v>1.180327868852459E-2</v>
+      </c>
+      <c r="N11" s="8">
         <f>D10/C10/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O11" s="8" t="e">
+        <v>1.3606557377049182E-2</v>
+      </c>
+      <c r="O11" s="8">
         <f>E11/B11/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="8" t="e">
+        <v>9.9180327868852464E-3</v>
+      </c>
+      <c r="P11" s="8">
         <f>E10/C10/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="8" t="e">
-        <f>B13/C13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S11" s="8" t="e">
+        <v>9.8360655737704927E-3</v>
+      </c>
+      <c r="R11" s="8">
+        <f>D13/C13</f>
+        <v>6.3549704947798462</v>
+      </c>
+      <c r="S11" s="8">
         <f>-B11/E11*1000</f>
-        <v>#DIV/0!</v>
+        <v>-100.82644628099173</v>
       </c>
       <c r="T11" s="8" t="e">
-        <f>D13/C13/1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U11" s="8" t="e">
+        <f>#REF!/C13/1000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="U11" s="8">
         <f>-D11/E11</f>
-        <v>#DIV/0!</v>
+        <v>-1.1900826446280992</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="24">
+        <f>2.557</f>
+        <v>2.5569999999999999</v>
+      </c>
+      <c r="C12" s="9">
+        <f>3.05</f>
+        <v>3.05</v>
+      </c>
       <c r="D12" s="9">
         <v>0</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9">
+        <f>32.5*0.5</f>
+        <v>16.25</v>
+      </c>
     </row>
     <row r="13" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="9">
+        <v>3.05</v>
+      </c>
+      <c r="C13" s="24">
+        <f>2.203</f>
+        <v>2.2029999999999998</v>
+      </c>
+      <c r="D13" s="9">
+        <f>28*0.5</f>
+        <v>14</v>
+      </c>
       <c r="E13" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="H15" s="21" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="H15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="23"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -1346,12 +1414,12 @@
       <c r="E16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="16"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -1404,19 +1472,19 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-      <c r="H20" s="12" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -1432,12 +1500,12 @@
       <c r="E21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
     </row>
     <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -1490,19 +1558,19 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16"/>
-      <c r="H25" s="10" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="H25" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
@@ -1518,12 +1586,12 @@
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
@@ -1576,19 +1644,19 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="H30" s="10" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
+      <c r="H30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
@@ -1604,12 +1672,12 @@
       <c r="E31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
@@ -1666,6 +1734,16 @@
     <sortCondition ref="O17:O24"/>
   </sortState>
   <mergeCells count="26">
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="A30:E30"/>
@@ -1682,16 +1760,6 @@
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1709,32 +1777,32 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
-      <c r="H1" s="20" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+      <c r="H1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
       <c r="L1" s="6"/>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="R1" s="10" t="s">
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="R1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -1750,28 +1818,28 @@
       <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11" t="str">
+      <c r="H2" s="13" t="str">
         <f>$A$1</f>
         <v xml:space="preserve">Cuadripolo "X" - Nro. De serie: xxxx </v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="11" t="str">
+      <c r="M2" s="13" t="str">
         <f>$A$1</f>
         <v xml:space="preserve">Cuadripolo "X" - Nro. De serie: xxxx </v>
       </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="R2" s="11" t="str">
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="R2" s="13" t="str">
         <f>$A$1</f>
         <v xml:space="preserve">Cuadripolo "X" - Nro. De serie: xxxx </v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">

</xml_diff>

<commit_message>
se te quema el cerebro
</commit_message>
<xml_diff>
--- a/TP5/Mediciones.xlsx
+++ b/TP5/Mediciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\Desktop\TP3 ELECTRO\TP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2818E8-B312-4ECB-AFDE-CFCE565734E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8CD6DA-0C1D-4B10-A4D9-F52DD00BBF8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FDA36349-2CEE-46F1-A8FD-45D31E04EF72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDA36349-2CEE-46F1-A8FD-45D31E04EF72}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="61">
   <si>
     <r>
       <t>V</t>
@@ -504,14 +504,191 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>P[W]</t>
+  </si>
+  <si>
+    <t>Equivalencias</t>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <t>Medido</t>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SERIE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PARALELO</t>
+    </r>
+  </si>
+  <si>
+    <t>Calculado</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CASCADA A-B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CASCADA B-A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B</t>
+    </r>
+  </si>
+  <si>
+    <t>Diferencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -536,7 +713,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,8 +750,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -647,11 +848,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,15 +899,45 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -710,34 +950,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1054,41 +1321,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1234583-11C2-4965-B267-EB43A84ACFA3}">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Z54"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51:N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="H1" s="31" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+      <c r="H1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
       <c r="L1" s="6"/>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="R1" s="15" t="s">
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="R1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -1104,28 +1375,28 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="16" t="str">
+      <c r="H2" s="15" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="16" t="str">
+      <c r="M2" s="15" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="R2" s="16" t="str">
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="R2" s="15" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
     </row>
     <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1290,31 +1561,31 @@
       <c r="F6" s="4"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="H8" s="18" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
+      <c r="H8" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="M8" s="17" t="s">
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="M8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="R8" s="15" t="s">
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="R8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
@@ -1330,27 +1601,27 @@
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="16" t="str">
+      <c r="H9" s="15" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="M9" s="16" t="str">
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="M9" s="15" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="R9" s="16" t="str">
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="R9" s="15" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1514,36 +1785,36 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="H15" s="22" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="H15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
-      <c r="N15" s="19" t="s">
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="19"/>
+      <c r="N15" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="R15" s="22" t="s">
+      <c r="O15" s="30"/>
+      <c r="P15" s="31"/>
+      <c r="R15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="24"/>
-      <c r="W15" s="22" t="s">
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="19"/>
+      <c r="W15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="24"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="19"/>
     </row>
     <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -1559,29 +1830,29 @@
       <c r="E16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="N16" s="19" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
+      <c r="N16" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
-      <c r="R16" s="25" t="s">
+      <c r="O16" s="30"/>
+      <c r="P16" s="31"/>
+      <c r="R16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="27"/>
-      <c r="W16" s="25" t="s">
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="22"/>
+      <c r="W16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="27"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="22"/>
     </row>
     <row r="17" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -1706,36 +1977,36 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="H20" s="17" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="H20" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="N20" s="19" t="s">
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="N20" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21"/>
-      <c r="R20" s="17" t="s">
+      <c r="O20" s="30"/>
+      <c r="P20" s="31"/>
+      <c r="R20" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="W20" s="17" t="s">
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="W20" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="X20" s="17"/>
-      <c r="Y20" s="17"/>
-      <c r="Z20" s="17"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
     </row>
     <row r="21" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -1751,24 +2022,24 @@
       <c r="E21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="R21" s="16" t="s">
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="R21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="W21" s="16" t="s">
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="W21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
     </row>
     <row r="22" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -1893,31 +2164,31 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="H25" s="15" t="s">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="H25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="R25" s="15" t="s">
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="R25" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="W25" s="15" t="s">
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="W25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
     </row>
     <row r="26" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
@@ -1933,24 +2204,24 @@
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="R26" s="16" t="s">
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="R26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="W26" s="16" t="s">
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="W26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
@@ -2074,31 +2345,31 @@
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="27"/>
-      <c r="H30" s="15" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="H30" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="R30" s="15" t="s">
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="R30" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="W30" s="15" t="s">
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="W30" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
+      <c r="X30" s="16"/>
+      <c r="Y30" s="16"/>
+      <c r="Z30" s="16"/>
     </row>
     <row r="31" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
@@ -2114,24 +2385,24 @@
       <c r="E31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="R31" s="16" t="s">
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="R31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
-      <c r="W31" s="16" t="s">
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="W31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="X31" s="16"/>
-      <c r="Y31" s="16"/>
-      <c r="Z31" s="16"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="15"/>
     </row>
     <row r="32" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
@@ -2253,25 +2524,546 @@
         <f t="shared" ref="Z33" si="11">ABS(K33-U33)</f>
         <v>2.2449022437907518</v>
       </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+    </row>
+    <row r="37" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="41"/>
+      <c r="C37" s="37">
+        <f>H4</f>
+        <v>371.95121951219505</v>
+      </c>
+      <c r="D37" s="37">
+        <f>I4</f>
+        <v>310.29411764705878</v>
+      </c>
+      <c r="E37" s="41"/>
+      <c r="F37" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="41"/>
+      <c r="H37" s="38">
+        <f>M4</f>
+        <v>5.4918032786885245E-3</v>
+      </c>
+      <c r="I37" s="38">
+        <f>N4</f>
+        <v>3.7704918032786887E-3</v>
+      </c>
+      <c r="J37" s="41"/>
+      <c r="K37" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="L37" s="41"/>
+      <c r="M37" s="38">
+        <f>R4</f>
+        <v>1.3958810068649885</v>
+      </c>
+      <c r="N37" s="38">
+        <f>S4</f>
+        <v>-265.21739130434781</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="37">
+        <f>J4</f>
+        <v>266.46341463414632</v>
+      </c>
+      <c r="D38" s="37">
+        <f>K4</f>
+        <v>448.5294117647058</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="38">
+        <f>O4</f>
+        <v>3.7704918032786887E-3</v>
+      </c>
+      <c r="I38" s="38">
+        <f>P4</f>
+        <v>5.2459016393442632E-3</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="38">
+        <f>T4</f>
+        <v>3.7528604118993139E-3</v>
+      </c>
+      <c r="N38" s="38">
+        <f>U4</f>
+        <v>-1.4565217391304348</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="40"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="40"/>
+    </row>
+    <row r="40" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="41"/>
+      <c r="C40" s="37">
+        <f>H11</f>
+        <v>217.85714285714283</v>
+      </c>
+      <c r="D40" s="37">
+        <f>I11</f>
+        <v>157.35384615384615</v>
+      </c>
+      <c r="E40" s="41"/>
+      <c r="F40" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="41"/>
+      <c r="H40" s="38">
+        <f>M11</f>
+        <v>1.180327868852459E-2</v>
+      </c>
+      <c r="I40" s="38">
+        <f>N11</f>
+        <v>1.3606557377049182E-2</v>
+      </c>
+      <c r="J40" s="41"/>
+      <c r="K40" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="L40" s="41"/>
+      <c r="M40" s="38">
+        <f>R11</f>
+        <v>6.3549704947798462</v>
+      </c>
+      <c r="N40" s="38">
+        <f>S11</f>
+        <v>-100.82644628099173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="41"/>
+      <c r="C41" s="37">
+        <f>J11</f>
+        <v>157.35714285714283</v>
+      </c>
+      <c r="D41" s="37">
+        <f>K11</f>
+        <v>187.69230769230768</v>
+      </c>
+      <c r="E41" s="41"/>
+      <c r="F41" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="41"/>
+      <c r="H41" s="38">
+        <f>O11</f>
+        <v>9.9180327868852464E-3</v>
+      </c>
+      <c r="I41" s="38">
+        <f>P11</f>
+        <v>9.8360655737704927E-3</v>
+      </c>
+      <c r="J41" s="41"/>
+      <c r="K41" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="L41" s="41"/>
+      <c r="M41" s="38">
+        <f>T11</f>
+        <v>6.3549704947798462E-3</v>
+      </c>
+      <c r="N41" s="38">
+        <f>U11</f>
+        <v>-1.1900826446280992</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B42" s="42"/>
+    </row>
+    <row r="43" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="42"/>
+      <c r="C43" s="37">
+        <f>H18</f>
+        <v>561.81818181818176</v>
+      </c>
+      <c r="D43" s="37">
+        <f>I18</f>
+        <v>605.88235294117646</v>
+      </c>
+      <c r="F43" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="42"/>
+      <c r="H43" s="45">
+        <f>C37+C40</f>
+        <v>589.80836236933783</v>
+      </c>
+      <c r="I43" s="45">
+        <f>D37+D40</f>
+        <v>467.6479638009049</v>
+      </c>
+      <c r="K43" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="L43" s="42"/>
+      <c r="M43" s="50">
+        <f>ABS(C43-H43)</f>
+        <v>27.990180551156072</v>
+      </c>
+      <c r="N43" s="50">
+        <f>ABS(D43-I43)</f>
+        <v>138.23438914027156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="42"/>
+      <c r="C44" s="37">
+        <f>J11</f>
+        <v>157.35714285714283</v>
+      </c>
+      <c r="D44" s="37">
+        <f>K11</f>
+        <v>187.69230769230768</v>
+      </c>
+      <c r="F44" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G44" s="42"/>
+      <c r="H44" s="45">
+        <f>C38+C41</f>
+        <v>423.82055749128915</v>
+      </c>
+      <c r="I44" s="45">
+        <f>D38+D41</f>
+        <v>636.22171945701348</v>
+      </c>
+      <c r="K44" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="L44" s="42"/>
+      <c r="M44" s="50">
+        <f>ABS(C44-H44)</f>
+        <v>266.46341463414632</v>
+      </c>
+      <c r="N44" s="50">
+        <f>ABS(D44-I44)</f>
+        <v>448.5294117647058</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="42"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="G45" s="42"/>
+      <c r="L45" s="42"/>
+    </row>
+    <row r="46" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="A46" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="42"/>
+      <c r="C46" s="38">
+        <f>H23</f>
+        <v>7.2815533980582527E-3</v>
+      </c>
+      <c r="D46" s="38">
+        <f>I23</f>
+        <v>1.3430420711974112E-2</v>
+      </c>
+      <c r="F46" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G46" s="42"/>
+      <c r="H46" s="47">
+        <f>H37+H40</f>
+        <v>1.7295081967213115E-2</v>
+      </c>
+      <c r="I46" s="47">
+        <f>I37+I40</f>
+        <v>1.7377049180327869E-2</v>
+      </c>
+      <c r="K46" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="L46" s="42"/>
+      <c r="M46" s="50">
+        <f>ABS(C46-H46)</f>
+        <v>1.0013528569154863E-2</v>
+      </c>
+      <c r="N46" s="50">
+        <f>ABS(D46-I46)</f>
+        <v>3.9466284683537575E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="42"/>
+      <c r="C47" s="38">
+        <f>J23</f>
+        <v>1.3430420711974112E-2</v>
+      </c>
+      <c r="D47" s="38">
+        <f>K23</f>
+        <v>1.8608414239482201E-3</v>
+      </c>
+      <c r="F47" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G47" s="42"/>
+      <c r="H47" s="47">
+        <f>H38+H41</f>
+        <v>1.3688524590163936E-2</v>
+      </c>
+      <c r="I47" s="47">
+        <f>I38+I41</f>
+        <v>1.5081967213114757E-2</v>
+      </c>
+      <c r="K47" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="L47" s="42"/>
+      <c r="M47" s="52">
+        <f>ABS(C47-H47)</f>
+        <v>2.5810387818982379E-4</v>
+      </c>
+      <c r="N47" s="50">
+        <f>ABS(D47-I47)</f>
+        <v>1.3221125789166536E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48" s="42"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="G48" s="42"/>
+      <c r="L48" s="42"/>
+    </row>
+    <row r="49" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A49" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="42"/>
+      <c r="C49" s="37">
+        <f>H28</f>
+        <v>2.2888888888888888</v>
+      </c>
+      <c r="D49" s="37">
+        <f>I28</f>
+        <v>-515</v>
+      </c>
+      <c r="F49" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="42"/>
+      <c r="H49" s="48">
+        <f t="array" ref="H49:I50">MMULT(M40:N41,M37:N38)</f>
+        <v>8.4923950341301602</v>
+      </c>
+      <c r="I49" s="48">
+        <v>-1538.5927855540797</v>
+      </c>
+      <c r="K49" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="L49" s="42"/>
+      <c r="M49" s="50">
+        <f>ABS(C49-H49)</f>
+        <v>6.2035061452412714</v>
+      </c>
+      <c r="N49" s="50">
+        <f>ABS(D49-I49)</f>
+        <v>1023.5927855540797</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="42"/>
+      <c r="C50" s="37">
+        <f>J28</f>
+        <v>1.3148148148148147E-2</v>
+      </c>
+      <c r="D50" s="37">
+        <f>K28</f>
+        <v>-3.4166666666666665</v>
+      </c>
+      <c r="F50" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G50" s="42"/>
+      <c r="H50" s="48">
+        <v>4.4045685689373523E-3</v>
+      </c>
+      <c r="I50" s="48">
+        <v>4.7932546821054967E-2</v>
+      </c>
+      <c r="K50" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="L50" s="42"/>
+      <c r="M50" s="50">
+        <f>ABS(C50-H50)</f>
+        <v>8.7435795792107952E-3</v>
+      </c>
+      <c r="N50" s="50">
+        <f>ABS(D50-I50)</f>
+        <v>3.4645992134877215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="42"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="G51" s="42"/>
+      <c r="L51" s="42"/>
+    </row>
+    <row r="52" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A52" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="42"/>
+      <c r="C52" s="37">
+        <f>H33</f>
+        <v>3.5558112773302644</v>
+      </c>
+      <c r="D52" s="37">
+        <f>I33</f>
+        <v>-468.18181818181813</v>
+      </c>
+      <c r="F52" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="G52" s="42"/>
+      <c r="H52" s="48">
+        <f t="array" ref="H52:I53">MMULT(M37:N38,M40:N41)</f>
+        <v>7.1853339164089753</v>
+      </c>
+      <c r="I52" s="48">
+        <v>174.88889309151426</v>
+      </c>
+      <c r="K52" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="L52" s="42"/>
+      <c r="M52" s="50">
+        <f>ABS(C52-H52)</f>
+        <v>3.629522639078711</v>
+      </c>
+      <c r="N52" s="50">
+        <f>ABS(D52-I52)</f>
+        <v>643.07071127333234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="42"/>
+      <c r="C53" s="38">
+        <f>J33</f>
+        <v>2.1359223300970879E-3</v>
+      </c>
+      <c r="D53" s="38">
+        <f>K33</f>
+        <v>-2.1969696969696968</v>
+      </c>
+      <c r="F53" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G53" s="42"/>
+      <c r="H53" s="48">
+        <v>1.4593164511468141E-2</v>
+      </c>
+      <c r="I53" s="48">
+        <v>1.3549936645422396</v>
+      </c>
+      <c r="K53" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="L53" s="42"/>
+      <c r="M53" s="50">
+        <f>ABS(C53-H53)</f>
+        <v>1.2457242181371054E-2</v>
+      </c>
+      <c r="N53" s="50">
+        <f>ABS(D53-I53)</f>
+        <v>3.5519633615119366</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="42"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M17:P24">
     <sortCondition ref="O17:O24"/>
   </sortState>
-  <mergeCells count="45">
-    <mergeCell ref="W26:Z26"/>
-    <mergeCell ref="W30:Z30"/>
-    <mergeCell ref="W31:Z31"/>
-    <mergeCell ref="W15:Z15"/>
-    <mergeCell ref="W16:Z16"/>
-    <mergeCell ref="W20:Z20"/>
-    <mergeCell ref="W21:Z21"/>
-    <mergeCell ref="W25:Z25"/>
-    <mergeCell ref="R21:U21"/>
-    <mergeCell ref="R25:U25"/>
-    <mergeCell ref="R26:U26"/>
-    <mergeCell ref="R30:U30"/>
-    <mergeCell ref="R31:U31"/>
+  <mergeCells count="46">
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="R20:U20"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="A30:E30"/>
@@ -2288,22 +3080,19 @@
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="R16:U16"/>
-    <mergeCell ref="R20:U20"/>
+    <mergeCell ref="R21:U21"/>
+    <mergeCell ref="R25:U25"/>
+    <mergeCell ref="R26:U26"/>
+    <mergeCell ref="R30:U30"/>
+    <mergeCell ref="R31:U31"/>
+    <mergeCell ref="W26:Z26"/>
+    <mergeCell ref="W30:Z30"/>
+    <mergeCell ref="W31:Z31"/>
+    <mergeCell ref="W15:Z15"/>
+    <mergeCell ref="W16:Z16"/>
+    <mergeCell ref="W20:Z20"/>
+    <mergeCell ref="W21:Z21"/>
+    <mergeCell ref="W25:Z25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2312,31 +3101,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC98DE4E-8D07-412A-8ADE-7579EC4BF84A}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="G1" s="28" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+      <c r="G1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="30"/>
-    </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -2367,8 +3157,11 @@
       <c r="K2" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>191.4</v>
       </c>
@@ -2400,8 +3193,12 @@
       <c r="K3" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="34">
+        <f>I3*J3</f>
+        <v>15.95825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2417,8 +3214,12 @@
       <c r="K4" s="9">
         <v>61.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="34">
+        <f t="shared" ref="L4:L8" si="0">I4*J4</f>
+        <v>16.9175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="13"/>
@@ -2432,8 +3233,12 @@
       <c r="K5" s="9">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="34">
+        <f t="shared" si="0"/>
+        <v>17.313500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -2447,8 +3252,12 @@
       <c r="K6" s="12">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="34">
+        <f t="shared" si="0"/>
+        <v>16.814999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -2462,8 +3271,12 @@
       <c r="K7" s="9">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="34">
+        <f t="shared" si="0"/>
+        <v>16.939999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -2477,11 +3290,15 @@
       <c r="K8" s="9">
         <v>120</v>
       </c>
+      <c r="L8" s="34">
+        <f t="shared" si="0"/>
+        <v>16.415000000000003</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
puto el que pullea
</commit_message>
<xml_diff>
--- a/TP5/Mediciones.xlsx
+++ b/TP5/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\Desktop\TP3 ELECTRO\TP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EBC3DE-9579-424A-8F98-3B8135095908}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EBB795-D329-43A4-9D7B-CA7219542594}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDA36349-2CEE-46F1-A8FD-45D31E04EF72}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <r>
       <t>V</t>
@@ -476,24 +476,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Parametro Z (Teórico)</t>
-  </si>
-  <si>
-    <t>Parametro Y  (Teórico)</t>
-  </si>
-  <si>
-    <t>Parametro T  (Teórico)</t>
-  </si>
-  <si>
-    <t>Parametro Z (Diferencia)</t>
-  </si>
-  <si>
-    <t>Parametro Y (Diferencia)</t>
-  </si>
-  <si>
-    <t>Parametro T (Diferencia)</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -727,6 +709,38 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> ^-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Con Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Con Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
     </r>
   </si>
 </sst>
@@ -734,9 +748,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -903,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -941,7 +956,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -974,67 +989,79 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1351,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1234583-11C2-4965-B267-EB43A84ACFA3}">
-  <dimension ref="A1:Z66"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:D65"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,35 +1390,35 @@
     <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="H1" s="38" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="H1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
       <c r="L1" s="6"/>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="R1" s="30" t="s">
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="R1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-    </row>
-    <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+    </row>
+    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1405,30 +1432,30 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="29" t="str">
+      <c r="H2" s="30" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="29" t="str">
+      <c r="M2" s="30" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="R2" s="29" t="str">
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="R2" s="30" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-    </row>
-    <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+    </row>
+    <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1484,7 +1511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1578,7 @@
         <v>-1.4565217391304348</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1570,7 +1597,7 @@
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1590,34 +1617,34 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="H8" s="43" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
+      <c r="H8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="M8" s="37" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="M8" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="R8" s="30" t="s">
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="R8" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
-    </row>
-    <row r="9" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+    </row>
+    <row r="9" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -1631,29 +1658,29 @@
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="29" t="str">
+      <c r="H9" s="30" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="M9" s="29" t="str">
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="M9" s="30" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="R9" s="29" t="str">
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="R9" s="30" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-    </row>
-    <row r="10" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+    </row>
+    <row r="10" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1696,19 +1723,19 @@
         <v>17</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1775,7 +1802,7 @@
         <v>-1.1900826446280992</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1795,7 +1822,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1814,39 +1841,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="H15" s="31" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="H15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33"/>
-      <c r="N15" s="44" t="s">
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
+      <c r="N15" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="45"/>
-      <c r="P15" s="46"/>
-      <c r="R15" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="33"/>
-      <c r="W15" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="X15" s="32"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="33"/>
-    </row>
-    <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="O15" s="34"/>
+      <c r="P15" s="35"/>
+    </row>
+    <row r="16" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>0</v>
@@ -1860,31 +1875,19 @@
       <c r="E16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="36"/>
-      <c r="N16" s="44" t="s">
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="41"/>
+      <c r="N16" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="O16" s="45"/>
-      <c r="P16" s="46"/>
-      <c r="R16" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="36"/>
-      <c r="W16" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="36"/>
-    </row>
-    <row r="17" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="O16" s="34"/>
+      <c r="P16" s="35"/>
+    </row>
+    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1914,32 +1917,8 @@
       <c r="K17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="U17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="W17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="X17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z17" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1973,72 +1952,28 @@
         <f>C18/E17*1000</f>
         <v>460.98039215686271</v>
       </c>
-      <c r="R18" s="14">
-        <f>H4+H11</f>
-        <v>589.80836236933783</v>
-      </c>
-      <c r="S18" s="14">
-        <f t="shared" ref="S18:U18" si="0">I4+I11</f>
-        <v>467.6479638009049</v>
-      </c>
-      <c r="T18" s="14">
-        <f t="shared" si="0"/>
-        <v>423.82055749128915</v>
-      </c>
-      <c r="U18" s="14">
-        <f t="shared" si="0"/>
-        <v>636.22171945701348</v>
-      </c>
-      <c r="W18" s="14">
-        <f>ABS(H18-R18)</f>
-        <v>27.990180551156072</v>
-      </c>
-      <c r="X18" s="14">
-        <f t="shared" ref="X18:Z18" si="1">ABS(I18-S18)</f>
-        <v>138.23438914027156</v>
-      </c>
-      <c r="Y18" s="14">
-        <f t="shared" si="1"/>
-        <v>3.6339879632563452</v>
-      </c>
-      <c r="Z18" s="14">
-        <f t="shared" si="1"/>
-        <v>175.24132730015077</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-      <c r="H20" s="37" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+      <c r="H20" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="N20" s="44" t="s">
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="N20" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="O20" s="45"/>
-      <c r="P20" s="46"/>
-      <c r="R20" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
-      <c r="W20" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
-    </row>
-    <row r="21" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="O20" s="34"/>
+      <c r="P20" s="35"/>
+    </row>
+    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
         <v>0</v>
@@ -2052,26 +1987,14 @@
       <c r="E21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="R21" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="W21" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="X21" s="29"/>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-    </row>
-    <row r="22" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -2101,32 +2024,8 @@
       <c r="K22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S22" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="W22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="X22" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z22" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -2160,67 +2059,23 @@
         <f>E22/1000/C22</f>
         <v>1.8608414239482201E-3</v>
       </c>
-      <c r="R23" s="8">
-        <f>M4+M11</f>
-        <v>1.7295081967213115E-2</v>
-      </c>
-      <c r="S23" s="8">
-        <f t="shared" ref="S23:U23" si="2">N4+N11</f>
-        <v>1.7377049180327869E-2</v>
-      </c>
-      <c r="T23" s="8">
-        <f t="shared" si="2"/>
-        <v>1.3688524590163936E-2</v>
-      </c>
-      <c r="U23" s="8">
-        <f t="shared" si="2"/>
-        <v>1.5081967213114757E-2</v>
-      </c>
-      <c r="W23" s="14">
-        <f>ABS(H23-R23)</f>
-        <v>1.0013528569154863E-2</v>
-      </c>
-      <c r="X23" s="14">
-        <f t="shared" ref="X23" si="3">ABS(I23-S23)</f>
-        <v>3.9466284683537575E-3</v>
-      </c>
-      <c r="Y23" s="14">
-        <f t="shared" ref="Y23" si="4">ABS(J23-T23)</f>
-        <v>2.5810387818982379E-4</v>
-      </c>
-      <c r="Z23" s="14">
-        <f t="shared" ref="Z23" si="5">ABS(K23-U23)</f>
-        <v>1.3221125789166536E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-      <c r="H25" s="30" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="41"/>
+      <c r="H25" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="R25" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="W25" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-    </row>
-    <row r="26" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+    </row>
+    <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
         <v>0</v>
@@ -2234,26 +2089,14 @@
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="29" t="s">
+      <c r="H26" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="R26" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="S26" s="29"/>
-      <c r="T26" s="29"/>
-      <c r="U26" s="29"/>
-      <c r="W26" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="X26" s="29"/>
-      <c r="Y26" s="29"/>
-      <c r="Z26" s="29"/>
-    </row>
-    <row r="27" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+    </row>
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -2283,32 +2126,8 @@
       <c r="K27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S27" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="T27" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="U27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="X27" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y27" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z27" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -2341,67 +2160,23 @@
         <f>-D27/E27</f>
         <v>-3.4166666666666665</v>
       </c>
-      <c r="R28" s="14">
-        <f>R4*R11+S4*T11</f>
-        <v>7.1853339164089753</v>
-      </c>
-      <c r="S28" s="14">
-        <f>R4*S11+S4*U11</f>
-        <v>174.88889309151426</v>
-      </c>
-      <c r="T28" s="14">
-        <f>T4*R11+U4*T11</f>
-        <v>1.4593164511468141E-2</v>
-      </c>
-      <c r="U28" s="14">
-        <f>T4*S11+U4*U11</f>
-        <v>1.3549936645422396</v>
-      </c>
-      <c r="W28" s="14">
-        <f>ABS(H28-R28)</f>
-        <v>4.8964450275200866</v>
-      </c>
-      <c r="X28" s="14">
-        <f t="shared" ref="X28" si="6">ABS(I28-S28)</f>
-        <v>689.88889309151432</v>
-      </c>
-      <c r="Y28" s="14">
-        <f t="shared" ref="Y28" si="7">ABS(J28-T28)</f>
-        <v>1.4450163633199942E-3</v>
-      </c>
-      <c r="Z28" s="14">
-        <f t="shared" ref="Z28" si="8">ABS(K28-U28)</f>
-        <v>4.7716603312089063</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
-      <c r="H30" s="30" t="s">
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="H30" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="R30" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="W30" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="30"/>
-      <c r="Z30" s="30"/>
-    </row>
-    <row r="31" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+    </row>
+    <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
         <v>0</v>
@@ -2415,26 +2190,14 @@
       <c r="E31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="29" t="s">
+      <c r="H31" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="R31" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="S31" s="29"/>
-      <c r="T31" s="29"/>
-      <c r="U31" s="29"/>
-      <c r="W31" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="X31" s="29"/>
-      <c r="Y31" s="29"/>
-      <c r="Z31" s="29"/>
-    </row>
-    <row r="32" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+    </row>
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -2464,32 +2227,8 @@
       <c r="K32" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R32" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="T32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="U32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W32" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="X32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z32" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -2522,55 +2261,28 @@
         <f>-D32/E32</f>
         <v>-2.1969696969696968</v>
       </c>
-      <c r="R33" s="14">
-        <f>R11*R4+S11*T4</f>
-        <v>8.4923950341301602</v>
-      </c>
-      <c r="S33" s="14">
-        <f>R11*S4+S11*U4</f>
-        <v>-1538.5927855540797</v>
-      </c>
-      <c r="T33" s="8">
-        <f>T11*R4+U11*T4</f>
-        <v>4.4045685689373523E-3</v>
-      </c>
-      <c r="U33" s="14">
-        <f>T11*S4+U11*U4</f>
-        <v>4.7932546821054967E-2</v>
-      </c>
-      <c r="W33" s="14">
-        <f>ABS(H33-R33)</f>
-        <v>4.9365837567998962</v>
-      </c>
-      <c r="X33" s="14">
-        <f t="shared" ref="X33" si="9">ABS(I33-S33)</f>
-        <v>1070.4109673722614</v>
-      </c>
-      <c r="Y33" s="14">
-        <f t="shared" ref="Y33" si="10">ABS(J33-T33)</f>
-        <v>2.2686462388402644E-3</v>
-      </c>
-      <c r="Z33" s="14">
-        <f t="shared" ref="Z33" si="11">ABS(K33-U33)</f>
-        <v>2.2449022437907518</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-    </row>
-    <row r="37" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
+    </row>
+    <row r="37" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="17">
@@ -2583,7 +2295,7 @@
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G37" s="21"/>
       <c r="H37" s="18">
@@ -2596,7 +2308,7 @@
       </c>
       <c r="J37" s="21"/>
       <c r="K37" s="16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="L37" s="21"/>
       <c r="M37" s="18">
@@ -2608,9 +2320,9 @@
         <v>-265.21739130434781</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="17">
@@ -2623,7 +2335,7 @@
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="18">
@@ -2636,7 +2348,7 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="18">
@@ -2648,7 +2360,7 @@
         <v>-1.4565217391304348</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
@@ -2664,9 +2376,9 @@
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
     </row>
-    <row r="40" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="17">
@@ -2679,7 +2391,7 @@
       </c>
       <c r="E40" s="21"/>
       <c r="F40" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G40" s="21"/>
       <c r="H40" s="18">
@@ -2692,7 +2404,7 @@
       </c>
       <c r="J40" s="21"/>
       <c r="K40" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="L40" s="21"/>
       <c r="M40" s="18">
@@ -2704,9 +2416,9 @@
         <v>-100.82644628099173</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="17">
@@ -2719,7 +2431,7 @@
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="18">
@@ -2732,7 +2444,7 @@
       </c>
       <c r="J41" s="21"/>
       <c r="K41" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L41" s="21"/>
       <c r="M41" s="18">
@@ -2744,12 +2456,12 @@
         <v>-1.1900826446280992</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="22"/>
     </row>
-    <row r="43" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B43" s="22"/>
       <c r="C43" s="17">
@@ -2761,7 +2473,7 @@
         <v>605.88235294117646</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="25">
@@ -2773,9 +2485,9 @@
         <v>467.6479638009049</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="17">
@@ -2787,7 +2499,7 @@
         <v>187.69230769230768</v>
       </c>
       <c r="F44" s="26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="25">
@@ -2799,16 +2511,16 @@
         <v>636.22171945701348</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="22"/>
       <c r="C45" s="23"/>
       <c r="D45" s="23"/>
       <c r="G45" s="22"/>
     </row>
-    <row r="46" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B46" s="22"/>
       <c r="C46" s="18">
@@ -2820,7 +2532,7 @@
         <v>1.3430420711974112E-2</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="27">
@@ -2832,9 +2544,9 @@
         <v>1.7377049180327869E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B47" s="22"/>
       <c r="C47" s="18">
@@ -2846,7 +2558,7 @@
         <v>1.8608414239482201E-3</v>
       </c>
       <c r="F47" s="26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="27">
@@ -2858,7 +2570,7 @@
         <v>1.5081967213114757E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
       <c r="B48" s="22"/>
       <c r="C48" s="23"/>
@@ -2867,7 +2579,7 @@
     </row>
     <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B49" s="22"/>
       <c r="C49" s="17">
@@ -2879,20 +2591,20 @@
         <v>-515</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="28">
         <f t="array" ref="H49:I50">MMULT(M40:N41,M37:N38)</f>
         <v>8.4923950341301602</v>
       </c>
-      <c r="I49" s="28">
+      <c r="I49" s="51">
         <v>-1538.5927855540797</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B50" s="22"/>
       <c r="C50" s="17">
@@ -2904,7 +2616,7 @@
         <v>-3.4166666666666665</v>
       </c>
       <c r="F50" s="26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="28">
@@ -2923,7 +2635,7 @@
     </row>
     <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B52" s="22"/>
       <c r="C52" s="17">
@@ -2935,20 +2647,20 @@
         <v>-468.18181818181813</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="28">
         <f t="array" ref="H52:I53">MMULT(M37:N38,M40:N41)</f>
         <v>7.1853339164089753</v>
       </c>
-      <c r="I52" s="28">
+      <c r="I52" s="52">
         <v>174.88889309151426</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B53" s="22"/>
       <c r="C53" s="18">
@@ -2960,7 +2672,7 @@
         <v>-2.1969696969696968</v>
       </c>
       <c r="F53" s="26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G53" s="22"/>
       <c r="H53" s="28">
@@ -2976,7 +2688,7 @@
     </row>
     <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="17">
@@ -2986,7 +2698,7 @@
         <v>310.29411764705878</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G55" s="21"/>
       <c r="H55" s="25">
@@ -2999,7 +2711,7 @@
     </row>
     <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="17">
@@ -3009,7 +2721,7 @@
         <v>448.5294117647058</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="25">
@@ -3028,7 +2740,7 @@
     </row>
     <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="17">
@@ -3038,7 +2750,7 @@
         <v>157.35384615384615</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G58" s="21"/>
       <c r="H58" s="25">
@@ -3051,7 +2763,7 @@
     </row>
     <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="17">
@@ -3061,7 +2773,7 @@
         <v>187.69230769230768</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G59" s="21"/>
       <c r="H59" s="25">
@@ -3076,7 +2788,7 @@
     </row>
     <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A61" s="16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="17">
@@ -3086,21 +2798,21 @@
         <v>-265.21739130434781</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="28">
         <f>C55/C56</f>
         <v>1.3958810068649885</v>
       </c>
-      <c r="I61" s="28">
-        <f>MDETERM(C55:D56)/C56</f>
-        <v>315.79956925561976</v>
+      <c r="I61" s="52">
+        <f>-MDETERM(C55:D56)/C56</f>
+        <v>-315.79956925561976</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A62" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="18">
@@ -3110,16 +2822,15 @@
         <v>-1.4565217391304348</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G62" s="22"/>
+        <v>56</v>
+      </c>
       <c r="H62" s="28">
         <f>1/C56</f>
         <v>3.7528604118993139E-3</v>
       </c>
-      <c r="I62" s="28">
-        <f>D56/C56</f>
-        <v>1.6832682729842507</v>
+      <c r="I62" s="52">
+        <f>-D56/C56</f>
+        <v>-1.6832682729842507</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3131,7 +2842,7 @@
     </row>
     <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="17">
@@ -3141,21 +2852,21 @@
         <v>-100.82644628099173</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G64" s="22"/>
-      <c r="H64" s="28">
+      <c r="H64" s="52">
         <f>C58/C59</f>
         <v>1.3844757149341806</v>
       </c>
-      <c r="I64" s="28">
-        <f>MDETERM(C58:D59)/C59</f>
-        <v>102.50159572610777</v>
+      <c r="I64" s="52">
+        <f>-MDETERM(C58:D59)/C59</f>
+        <v>-102.50159572610777</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A65" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="17">
@@ -3165,16 +2876,15 @@
         <v>-1.1900826446280992</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G65" s="22"/>
-      <c r="H65" s="28">
+        <v>57</v>
+      </c>
+      <c r="H65" s="52">
         <f>1/C59</f>
         <v>6.354970494779847E-3</v>
       </c>
-      <c r="I65" s="28">
-        <f>D59/C59</f>
-        <v>1.1927790774817557</v>
+      <c r="I65" s="52">
+        <f>-D59/C59</f>
+        <v>-1.1927790774817557</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3184,8 +2894,24 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M17:P24">
     <sortCondition ref="O17:O24"/>
   </sortState>
-  <mergeCells count="46">
-    <mergeCell ref="A35:I35"/>
+  <mergeCells count="30">
+    <mergeCell ref="A35:N35"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H25:K25"/>
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="R2:U2"/>
@@ -3199,38 +2925,6 @@
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="N20:P20"/>
     <mergeCell ref="N16:P16"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="R16:U16"/>
-    <mergeCell ref="R20:U20"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="R21:U21"/>
-    <mergeCell ref="R25:U25"/>
-    <mergeCell ref="R26:U26"/>
-    <mergeCell ref="R30:U30"/>
-    <mergeCell ref="R31:U31"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="W26:Z26"/>
-    <mergeCell ref="W30:Z30"/>
-    <mergeCell ref="W31:Z31"/>
-    <mergeCell ref="W15:Z15"/>
-    <mergeCell ref="W16:Z16"/>
-    <mergeCell ref="W20:Z20"/>
-    <mergeCell ref="W21:Z21"/>
-    <mergeCell ref="W25:Z25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3248,21 +2942,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="G1" s="47" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="G1" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3296,7 +2990,7 @@
         <v>33</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
PUTO EL QUE LEE (perdí)
</commit_message>
<xml_diff>
--- a/TP5/Mediciones.xlsx
+++ b/TP5/Mediciones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\Desktop\TP3 ELECTRO\TP5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EBB795-D329-43A4-9D7B-CA7219542594}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B69C04C-B395-4411-9333-6F4153D940E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDA36349-2CEE-46F1-A8FD-45D31E04EF72}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="58">
   <si>
     <r>
       <t>V</t>
@@ -821,13 +821,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -971,36 +971,71 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1013,55 +1048,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1378,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1234583-11C2-4965-B267-EB43A84ACFA3}">
-  <dimension ref="A1:U66"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,32 +1390,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
-      <c r="H1" s="42" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="6"/>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="R1" s="29" t="s">
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="R1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
     </row>
     <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -1432,28 +1431,28 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="30" t="str">
+      <c r="H2" s="34" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="30" t="str">
+      <c r="M2" s="34" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="R2" s="30" t="str">
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="R2" s="34" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1618,31 +1617,31 @@
       <c r="F6" s="4"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
-      <c r="H8" s="32" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="H8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="M8" s="31" t="s">
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="M8" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="R8" s="29" t="s">
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="R8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="42"/>
     </row>
     <row r="9" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
@@ -1658,27 +1657,27 @@
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="30" t="str">
+      <c r="H9" s="34" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="M9" s="30" t="str">
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="M9" s="34" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="R9" s="30" t="str">
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="R9" s="34" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
     </row>
     <row r="10" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -1842,24 +1841,24 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="H15" s="36" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="H15" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
-      <c r="N15" s="33" t="s">
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
+      <c r="N15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="34"/>
-      <c r="P15" s="35"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="46"/>
     </row>
     <row r="16" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -1875,17 +1874,17 @@
       <c r="E16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
-      <c r="N16" s="33" t="s">
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="32"/>
+      <c r="N16" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="O16" s="34"/>
-      <c r="P16" s="35"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="46"/>
     </row>
     <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -1954,24 +1953,24 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
-      <c r="H20" s="31" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="H20" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="N20" s="33" t="s">
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="N20" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="O20" s="34"/>
-      <c r="P20" s="35"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="46"/>
     </row>
     <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -1987,12 +1986,12 @@
       <c r="E21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -2061,19 +2060,19 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="H25" s="29" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
+      <c r="H25" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
     </row>
     <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
@@ -2089,12 +2088,12 @@
       <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="30" t="s">
+      <c r="H26" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
     </row>
     <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
@@ -2162,19 +2161,19 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
-      <c r="H30" s="29" t="s">
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="32"/>
+      <c r="H30" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
     </row>
     <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
@@ -2190,12 +2189,12 @@
       <c r="E31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="30" t="s">
+      <c r="H31" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
     </row>
     <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
@@ -2228,7 +2227,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -2262,639 +2261,481 @@
         <v>-2.1969696969696968</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="48" t="s">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="50"/>
-    </row>
-    <row r="37" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="51"/>
+    </row>
+    <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="18">
+        <f>M4</f>
+        <v>5.4918032786885245E-3</v>
+      </c>
+      <c r="C37" s="18">
+        <f>N4</f>
+        <v>3.7704918032786887E-3</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="18">
+        <f>M11</f>
+        <v>1.180327868852459E-2</v>
+      </c>
+      <c r="G37" s="18">
+        <f>N11</f>
+        <v>1.3606557377049182E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="18">
+        <f>O4</f>
+        <v>3.7704918032786887E-3</v>
+      </c>
+      <c r="C38" s="18">
+        <f>P4</f>
+        <v>5.2459016393442632E-3</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="18">
+        <f>O11</f>
+        <v>9.9180327868852464E-3</v>
+      </c>
+      <c r="G38" s="18">
+        <f>P11</f>
+        <v>9.8360655737704927E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="20"/>
+    </row>
+    <row r="40" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="17">
+      <c r="B40" s="17">
         <f>H4</f>
         <v>371.95121951219505</v>
       </c>
-      <c r="D37" s="17">
+      <c r="C40" s="17">
         <f>I4</f>
         <v>310.29411764705878</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" s="21"/>
-      <c r="H37" s="18">
-        <f>M4</f>
-        <v>5.4918032786885245E-3</v>
-      </c>
-      <c r="I37" s="18">
-        <f>N4</f>
-        <v>3.7704918032786887E-3</v>
-      </c>
-      <c r="J37" s="21"/>
-      <c r="K37" s="16" t="s">
+      <c r="D40" s="20"/>
+      <c r="E40" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="24">
+        <f t="array" ref="F40:G41">MINVERSE(B37:C38)</f>
+        <v>359.48434622467772</v>
+      </c>
+      <c r="G40" s="24">
+        <v>-258.37937384898709</v>
+      </c>
+      <c r="I40" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="L37" s="21"/>
-      <c r="M37" s="18">
+      <c r="J40" s="18">
         <f>R4</f>
         <v>1.3958810068649885</v>
       </c>
-      <c r="N37" s="18">
+      <c r="K40" s="18">
         <f>S4</f>
         <v>-265.21739130434781</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="M40" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N40" s="27">
+        <f>B40/B41</f>
+        <v>1.3958810068649885</v>
+      </c>
+      <c r="O40" s="29">
+        <f>MDETERM(B40:C41)/B41</f>
+        <v>315.79956925561976</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="17">
+      <c r="B41" s="17">
         <f>J4</f>
         <v>266.46341463414632</v>
       </c>
-      <c r="D38" s="17">
+      <c r="C41" s="17">
         <f>K4</f>
         <v>448.5294117647058</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="19" t="s">
+      <c r="D41" s="4"/>
+      <c r="E41" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="24">
+        <v>-258.37937384898709</v>
+      </c>
+      <c r="G41" s="24">
+        <v>376.33517495395944</v>
+      </c>
+      <c r="I41" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="18">
-        <f>O4</f>
-        <v>3.7704918032786887E-3</v>
-      </c>
-      <c r="I38" s="18">
-        <f>P4</f>
-        <v>5.2459016393442632E-3</v>
-      </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="L38" s="4"/>
-      <c r="M38" s="18">
+      <c r="J41" s="18">
         <f>T4</f>
         <v>3.7528604118993139E-3</v>
       </c>
-      <c r="N38" s="18">
+      <c r="K41" s="18">
         <f>U4</f>
         <v>-1.4565217391304348</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-    </row>
-    <row r="40" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A40" s="16" t="s">
+      <c r="M41" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="N41" s="27">
+        <f>1/B41</f>
+        <v>3.7528604118993139E-3</v>
+      </c>
+      <c r="O41" s="29">
+        <f>C41/B41</f>
+        <v>1.6832682729842507</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="20"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+    </row>
+    <row r="43" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="17">
+      <c r="B43" s="17">
         <f>H11</f>
         <v>217.85714285714283</v>
       </c>
-      <c r="D40" s="17">
+      <c r="C43" s="17">
         <f>I11</f>
         <v>157.35384615384615</v>
       </c>
-      <c r="E40" s="21"/>
-      <c r="F40" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G40" s="21"/>
-      <c r="H40" s="18">
-        <f>M11</f>
-        <v>1.180327868852459E-2</v>
-      </c>
-      <c r="I40" s="18">
-        <f>N11</f>
-        <v>1.3606557377049182E-2</v>
-      </c>
-      <c r="J40" s="21"/>
-      <c r="K40" s="16" t="s">
+      <c r="D43" s="20"/>
+      <c r="E43" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="24">
+        <f t="array" ref="F43:G44">MINVERSE(F37:G38)</f>
+        <v>-521.73913043478262</v>
+      </c>
+      <c r="G43" s="24">
+        <v>721.73913043478262</v>
+      </c>
+      <c r="I43" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="L40" s="21"/>
-      <c r="M40" s="18">
+      <c r="J43" s="18">
         <f>R11</f>
         <v>6.3549704947798462</v>
       </c>
-      <c r="N40" s="18">
+      <c r="K43" s="18">
         <f>S11</f>
         <v>-100.82644628099173</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="M43" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="N43" s="27">
+        <f>B43/B44</f>
+        <v>1.3844757149341806</v>
+      </c>
+      <c r="O43" s="29">
+        <f>MDETERM(B43:C44)/B44</f>
+        <v>102.50159572610777</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A44" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="17">
+      <c r="B44" s="17">
         <f>J11</f>
         <v>157.35714285714283</v>
       </c>
-      <c r="D41" s="17">
+      <c r="C44" s="17">
         <f>K11</f>
         <v>187.69230769230768</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="19" t="s">
+      <c r="D44" s="20"/>
+      <c r="E44" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="24">
+        <v>526.08695652173913</v>
+      </c>
+      <c r="G44" s="24">
+        <v>-626.08695652173913</v>
+      </c>
+      <c r="I44" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="21"/>
-      <c r="H41" s="18">
-        <f>O11</f>
-        <v>9.9180327868852464E-3</v>
-      </c>
-      <c r="I41" s="18">
-        <f>P11</f>
-        <v>9.8360655737704927E-3</v>
-      </c>
-      <c r="J41" s="21"/>
-      <c r="K41" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="L41" s="21"/>
-      <c r="M41" s="18">
+      <c r="J44" s="18">
         <f>T11</f>
         <v>6.3549704947798462E-3</v>
       </c>
-      <c r="N41" s="18">
+      <c r="K44" s="18">
         <f>U11</f>
         <v>-1.1900826446280992</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="22"/>
-    </row>
-    <row r="43" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
+      <c r="M44" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="N44" s="27">
+        <f>1/B44</f>
+        <v>6.354970494779847E-3</v>
+      </c>
+      <c r="O44" s="29">
+        <f>C44/B44</f>
+        <v>1.1927790774817557</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A46" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="17">
+      <c r="B46" s="17">
         <f>H18</f>
         <v>561.81818181818176</v>
       </c>
-      <c r="D43" s="17">
+      <c r="C46" s="17">
         <f>I18</f>
         <v>605.88235294117646</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="E46" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="22"/>
-      <c r="H43" s="25">
-        <f>C37+C40</f>
+      <c r="F46" s="24">
+        <f>B40+B43</f>
         <v>589.80836236933783</v>
       </c>
-      <c r="I43" s="25">
-        <f>D37+D40</f>
+      <c r="G46" s="24">
+        <f>C40+C43</f>
         <v>467.6479638009049</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="I46" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J46" s="17">
+        <f>H28</f>
+        <v>2.2888888888888888</v>
+      </c>
+      <c r="K46" s="17">
+        <f>I28</f>
+        <v>-515</v>
+      </c>
+      <c r="M46" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="N46" s="27">
+        <f t="array" ref="N46:O47">MMULT(J43:K44,J40:K41)</f>
+        <v>8.4923950341301602</v>
+      </c>
+      <c r="O46" s="28">
+        <v>-1538.5927855540797</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="17">
+      <c r="B47" s="17">
         <f>J11</f>
         <v>157.35714285714283</v>
       </c>
-      <c r="D44" s="17">
+      <c r="C47" s="17">
         <f>K11</f>
         <v>187.69230769230768</v>
       </c>
-      <c r="F44" s="26" t="s">
+      <c r="E47" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G44" s="22"/>
-      <c r="H44" s="25">
-        <f>C38+C41</f>
+      <c r="F47" s="24">
+        <f>B41+B44</f>
         <v>423.82055749128915</v>
       </c>
-      <c r="I44" s="25">
-        <f>D38+D41</f>
+      <c r="G47" s="24">
+        <f>C41+C44</f>
         <v>636.22171945701348</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="G45" s="22"/>
-    </row>
-    <row r="46" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A46" s="16" t="s">
+      <c r="I47" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="17">
+        <f>J28</f>
+        <v>1.3148148148148147E-2</v>
+      </c>
+      <c r="K47" s="17">
+        <f>K28</f>
+        <v>-3.4166666666666665</v>
+      </c>
+      <c r="M47" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="N47" s="27">
+        <v>4.4045685689373523E-3</v>
+      </c>
+      <c r="O47" s="27">
+        <v>4.7932546821054967E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+    </row>
+    <row r="49" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A49" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="18">
+      <c r="B49" s="18">
         <f>H23</f>
         <v>7.2815533980582527E-3</v>
       </c>
-      <c r="D46" s="18">
+      <c r="C49" s="18">
         <f>I23</f>
         <v>1.3430420711974112E-2</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="E49" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="22"/>
-      <c r="H46" s="27">
-        <f>H37+H40</f>
+      <c r="F49" s="26">
+        <f>B37+F37</f>
         <v>1.7295081967213115E-2</v>
       </c>
-      <c r="I46" s="27">
-        <f>I37+I40</f>
+      <c r="G49" s="26">
+        <f>C37+G37</f>
         <v>1.7377049180327869E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="I49" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J49" s="17">
+        <f>H33</f>
+        <v>3.5558112773302644</v>
+      </c>
+      <c r="K49" s="17">
+        <f>I33</f>
+        <v>-468.18181818181813</v>
+      </c>
+      <c r="M49" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="N49" s="27">
+        <f t="array" ref="N49:O50">MMULT(J40:K41,J43:K44)</f>
+        <v>7.1853339164089753</v>
+      </c>
+      <c r="O49" s="29">
+        <v>174.88889309151426</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="18">
+      <c r="B50" s="18">
         <f>J23</f>
         <v>1.3430420711974112E-2</v>
       </c>
-      <c r="D47" s="18">
+      <c r="C50" s="18">
         <f>K23</f>
         <v>1.8608414239482201E-3</v>
       </c>
-      <c r="F47" s="26" t="s">
+      <c r="E50" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G47" s="22"/>
-      <c r="H47" s="27">
-        <f>H38+H41</f>
+      <c r="F50" s="26">
+        <f>B38+F38</f>
         <v>1.3688524590163936E-2</v>
       </c>
-      <c r="I47" s="27">
-        <f>I38+I41</f>
+      <c r="G50" s="26">
+        <f>C38+G38</f>
         <v>1.5081967213114757E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A49" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="17">
-        <f>H28</f>
-        <v>2.2888888888888888</v>
-      </c>
-      <c r="D49" s="17">
-        <f>I28</f>
-        <v>-515</v>
-      </c>
-      <c r="F49" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="G49" s="22"/>
-      <c r="H49" s="28">
-        <f t="array" ref="H49:I50">MMULT(M40:N41,M37:N38)</f>
-        <v>8.4923950341301602</v>
-      </c>
-      <c r="I49" s="51">
-        <v>-1538.5927855540797</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="I50" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="17">
-        <f>J28</f>
-        <v>1.3148148148148147E-2</v>
-      </c>
-      <c r="D50" s="17">
-        <f>K28</f>
-        <v>-3.4166666666666665</v>
-      </c>
-      <c r="F50" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G50" s="22"/>
-      <c r="H50" s="28">
-        <v>4.4045685689373523E-3</v>
-      </c>
-      <c r="I50" s="28">
-        <v>4.7932546821054967E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="G51" s="22"/>
-    </row>
-    <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A52" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="17">
-        <f>H33</f>
-        <v>3.5558112773302644</v>
-      </c>
-      <c r="D52" s="17">
-        <f>I33</f>
-        <v>-468.18181818181813</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G52" s="22"/>
-      <c r="H52" s="28">
-        <f t="array" ref="H52:I53">MMULT(M37:N38,M40:N41)</f>
-        <v>7.1853339164089753</v>
-      </c>
-      <c r="I52" s="52">
-        <v>174.88889309151426</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="18">
+      <c r="J50" s="18">
         <f>J33</f>
         <v>2.1359223300970879E-3</v>
       </c>
-      <c r="D53" s="18">
+      <c r="K50" s="18">
         <f>K33</f>
         <v>-2.1969696969696968</v>
       </c>
-      <c r="F53" s="26" t="s">
+      <c r="M50" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G53" s="22"/>
-      <c r="H53" s="28">
+      <c r="N50" s="27">
         <v>1.4593164511468141E-2</v>
       </c>
-      <c r="I53" s="28">
+      <c r="O50" s="27">
         <v>1.3549936645422396</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="22"/>
-      <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A55" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="17">
-        <v>371.95121951219505</v>
-      </c>
-      <c r="D55" s="17">
-        <v>310.29411764705878</v>
-      </c>
-      <c r="F55" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G55" s="21"/>
-      <c r="H55" s="25">
-        <f t="array" ref="H55:I56">MINVERSE(H37:I38)</f>
-        <v>359.48434622467772</v>
-      </c>
-      <c r="I55" s="25">
-        <v>-258.37937384898709</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A56" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="17">
-        <v>266.46341463414632</v>
-      </c>
-      <c r="D56" s="17">
-        <v>448.5294117647058</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G56" s="4"/>
-      <c r="H56" s="25">
-        <v>-258.37937384898709</v>
-      </c>
-      <c r="I56" s="25">
-        <v>376.33517495395944</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="G57" s="22"/>
-    </row>
-    <row r="58" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A58" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="17">
-        <v>217.85714285714283</v>
-      </c>
-      <c r="D58" s="17">
-        <v>157.35384615384615</v>
-      </c>
-      <c r="F58" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="G58" s="21"/>
-      <c r="H58" s="25">
-        <f t="array" ref="H58:I59">MINVERSE(H40:I41)</f>
-        <v>-521.73913043478262</v>
-      </c>
-      <c r="I58" s="25">
-        <v>721.73913043478262</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="17">
-        <v>157.35714285714283</v>
-      </c>
-      <c r="D59" s="17">
-        <v>187.69230769230768</v>
-      </c>
-      <c r="F59" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G59" s="21"/>
-      <c r="H59" s="25">
-        <v>526.08695652173913</v>
-      </c>
-      <c r="I59" s="25">
-        <v>-626.08695652173913</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A61" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B61" s="21"/>
-      <c r="C61" s="17">
-        <v>1.3958810068649885</v>
-      </c>
-      <c r="D61" s="17">
-        <v>-265.21739130434781</v>
-      </c>
-      <c r="F61" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="G61" s="22"/>
-      <c r="H61" s="28">
-        <f>C55/C56</f>
-        <v>1.3958810068649885</v>
-      </c>
-      <c r="I61" s="52">
-        <f>-MDETERM(C55:D56)/C56</f>
-        <v>-315.79956925561976</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A62" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="18">
-        <v>3.7528604118993139E-3</v>
-      </c>
-      <c r="D62" s="17">
-        <v>-1.4565217391304348</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H62" s="28">
-        <f>1/C56</f>
-        <v>3.7528604118993139E-3</v>
-      </c>
-      <c r="I62" s="52">
-        <f>-D56/C56</f>
-        <v>-1.6832682729842507</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="G63" s="22"/>
-    </row>
-    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A64" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B64" s="21"/>
-      <c r="C64" s="17">
-        <v>6.3549704947798462</v>
-      </c>
-      <c r="D64" s="17">
-        <v>-100.82644628099173</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="G64" s="22"/>
-      <c r="H64" s="52">
-        <f>C58/C59</f>
-        <v>1.3844757149341806</v>
-      </c>
-      <c r="I64" s="52">
-        <f>-MDETERM(C58:D59)/C59</f>
-        <v>-102.50159572610777</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A65" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" s="21"/>
-      <c r="C65" s="17">
-        <v>6.3549704947798462E-3</v>
-      </c>
-      <c r="D65" s="17">
-        <v>-1.1900826446280992</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H65" s="52">
-        <f>1/C59</f>
-        <v>6.354970494779847E-3</v>
-      </c>
-      <c r="I65" s="52">
-        <f>-D59/C59</f>
-        <v>-1.1927790774817557</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G66" s="22"/>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M17:P24">
     <sortCondition ref="O17:O24"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N16:P16"/>
     <mergeCell ref="A35:N35"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H1:K1"/>
@@ -2911,20 +2752,6 @@
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="N16:P16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2942,21 +2769,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
-      <c r="G1" s="46" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="G1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Estoy en clases con tato! HELP ME!
</commit_message>
<xml_diff>
--- a/TP5/Mediciones.xlsx
+++ b/TP5/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\Desktop\TP3 ELECTRO\TP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9CFC44-542B-4288-93BB-06469607236C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD00522-CE14-4EB4-B47A-A5C6757AFC91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDA36349-2CEE-46F1-A8FD-45D31E04EF72}"/>
   </bookViews>
@@ -778,7 +778,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -796,6 +796,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1017,54 +1025,6 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1097,34 +1057,67 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,25 +1127,40 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1471,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1234583-11C2-4965-B267-EB43A84ACFA3}">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,32 +1490,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="H1" s="28" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
+      <c r="H1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="R1" s="31" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="R1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
     </row>
     <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -1523,28 +1531,28 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="29" t="str">
+      <c r="H2" s="42" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="29" t="str">
+      <c r="M2" s="42" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="R2" s="29" t="str">
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="R2" s="42" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
     </row>
     <row r="3" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -1564,18 +1572,18 @@
         <f>32*0.5</f>
         <v>16</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="34" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="4"/>
@@ -1622,8 +1630,8 @@
         <f>0.5*23</f>
         <v>11.5</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="13">
         <f>B6/D6*1000</f>
         <v>371.95121951219505</v>
@@ -1656,7 +1664,7 @@
         <f>E3/C3/1000</f>
         <v>5.2459016393442632E-3</v>
       </c>
-      <c r="Q4" s="40"/>
+      <c r="Q4" s="24"/>
       <c r="R4" s="7">
         <f>B6/C6</f>
         <v>1.3958810068649885</v>
@@ -1692,21 +1700,21 @@
         <f>0.1*68</f>
         <v>6.8000000000000007</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
     </row>
     <row r="6" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
@@ -1726,77 +1734,77 @@
       <c r="E6" s="13">
         <v>0</v>
       </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="40"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="55" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="M8" s="68" t="s">
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="M8" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="69" t="s">
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
     </row>
     <row r="9" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="56"/>
-      <c r="B9" s="57" t="s">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1808,30 +1816,30 @@
       <c r="E9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="58" t="str">
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="56" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="M9" s="70" t="str">
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="M9" s="44" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="70" t="str">
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="44" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
     </row>
     <row r="10" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
@@ -1851,43 +1859,43 @@
         <f>60*0.5</f>
         <v>30</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="50" t="s">
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="50" t="s">
+      <c r="I10" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="50" t="s">
+      <c r="K10" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="71" t="s">
+      <c r="M10" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="71" t="s">
+      <c r="N10" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="71" t="s">
+      <c r="O10" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="P10" s="71" t="s">
+      <c r="P10" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="71" t="s">
+      <c r="Q10" s="24"/>
+      <c r="R10" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="S10" s="71" t="s">
+      <c r="S10" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="T10" s="71" t="s">
+      <c r="T10" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="U10" s="71" t="s">
+      <c r="U10" s="39" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1909,8 +1917,8 @@
         <f>60.5*0.5</f>
         <v>30.25</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="13">
         <f>B13/D13*1000</f>
         <v>217.85714285714283</v>
@@ -1943,7 +1951,7 @@
         <f>E10/C10/1000</f>
         <v>9.8360655737704927E-3</v>
       </c>
-      <c r="Q11" s="40"/>
+      <c r="Q11" s="24"/>
       <c r="R11" s="7">
         <f>D13/C13</f>
         <v>6.3549704947798462</v>
@@ -1980,12 +1988,12 @@
         <f>32.5*0.5</f>
         <v>16.25</v>
       </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
@@ -2005,51 +2013,51 @@
       <c r="E13" s="13">
         <v>0</v>
       </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
     </row>
     <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="62" t="s">
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="64"/>
-      <c r="N15" s="37" t="s">
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
+      <c r="N15" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
     </row>
     <row r="16" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="57" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -2061,25 +2069,25 @@
       <c r="E16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="59" t="s">
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="61"/>
-      <c r="N16" s="32" t="s">
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="54"/>
+      <c r="N16" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="33"/>
-      <c r="P16" s="34"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="50"/>
     </row>
     <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="65">
+      <c r="B17" s="38">
         <f>2.158</f>
         <v>2.1579999999999999</v>
       </c>
@@ -2093,25 +2101,25 @@
         <f>51*0.1</f>
         <v>5.1000000000000005</v>
       </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="50" t="s">
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="50" t="s">
+      <c r="I17" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="50" t="s">
+      <c r="J17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="50" t="s">
+      <c r="K17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="N17" s="32" t="s">
+      <c r="N17" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="33"/>
-      <c r="P17" s="34"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="50"/>
     </row>
     <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
@@ -2131,8 +2139,8 @@
       <c r="E18" s="13">
         <v>0</v>
       </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
       <c r="H18" s="13">
         <f>B18/D18*1000</f>
         <v>561.81818181818176</v>
@@ -2151,43 +2159,43 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="66" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="66"/>
-      <c r="N20" s="32" t="s">
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="N20" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="O20" s="33"/>
-      <c r="P20" s="34"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="50"/>
     </row>
     <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="56"/>
-      <c r="B21" s="57" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -2199,14 +2207,14 @@
       <c r="E21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="58" t="s">
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
@@ -2226,18 +2234,18 @@
         <f>0.25*23</f>
         <v>5.75</v>
       </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50" t="s">
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="50" t="s">
+      <c r="I22" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="50" t="s">
+      <c r="J22" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="50" t="s">
+      <c r="K22" s="34" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2259,8 +2267,8 @@
         <f>83*0.5</f>
         <v>41.5</v>
       </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
       <c r="H23" s="13">
         <f>D23/1000/B23</f>
         <v>7.2815533980582527E-3</v>
@@ -2279,38 +2287,38 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="67" t="s">
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
     </row>
     <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="56"/>
-      <c r="B26" s="57" t="s">
+      <c r="A26" s="36"/>
+      <c r="B26" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -2322,14 +2330,14 @@
       <c r="E26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="58" t="s">
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
     </row>
     <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
@@ -2349,18 +2357,18 @@
         <f>0.1*60</f>
         <v>6</v>
       </c>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="50" t="s">
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="50" t="s">
+      <c r="I27" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="K27" s="50" t="s">
+      <c r="K27" s="34" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2381,8 +2389,8 @@
       <c r="E28" s="13">
         <v>0</v>
       </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
       <c r="H28" s="13">
         <f>B28/C28</f>
         <v>2.2888888888888888</v>
@@ -2401,38 +2409,38 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="59" t="s">
+      <c r="A30" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="67" t="s">
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="56"/>
-      <c r="B31" s="57" t="s">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -2444,14 +2452,14 @@
       <c r="E31" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="58" t="s">
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
     </row>
     <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
@@ -2471,18 +2479,18 @@
         <f>0.1*66</f>
         <v>6.6000000000000005</v>
       </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="50" t="s">
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="50" t="s">
+      <c r="I32" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="50" t="s">
+      <c r="J32" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="K32" s="50" t="s">
+      <c r="K32" s="34" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2503,8 +2511,8 @@
       <c r="E33" s="13">
         <v>0</v>
       </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
       <c r="H33" s="13">
         <f>B33/C33</f>
         <v>3.5558112773302644</v>
@@ -2523,22 +2531,23 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="24"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="70"/>
+      <c r="M35" s="70"/>
+      <c r="N35" s="70"/>
+      <c r="O35" s="71"/>
     </row>
     <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="19" t="s">
@@ -2552,8 +2561,8 @@
         <f>N4</f>
         <v>3.7704918032786887E-3</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="39" t="s">
+      <c r="D37" s="22"/>
+      <c r="E37" s="23" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="18">
@@ -2564,14 +2573,14 @@
         <f>N11</f>
         <v>1.3606557377049182E-2</v>
       </c>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="40"/>
-      <c r="N37" s="40"/>
-      <c r="O37" s="40"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
@@ -2585,8 +2594,8 @@
         <f>P4</f>
         <v>5.2459016393442632E-3</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="42" t="s">
+      <c r="D38" s="25"/>
+      <c r="E38" s="26" t="s">
         <v>43</v>
       </c>
       <c r="F38" s="18">
@@ -2597,31 +2606,31 @@
         <f>P11</f>
         <v>9.8360655737704927E-3</v>
       </c>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="O38" s="40"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="44"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
     </row>
     <row r="40" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="19" t="s">
@@ -2635,8 +2644,8 @@
         <f>I4</f>
         <v>310.29411764705878</v>
       </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="45" t="s">
+      <c r="D40" s="22"/>
+      <c r="E40" s="29" t="s">
         <v>44</v>
       </c>
       <c r="F40" s="21">
@@ -2646,8 +2655,8 @@
       <c r="G40" s="17">
         <v>-258.37937384898709</v>
       </c>
-      <c r="H40" s="40"/>
-      <c r="I40" s="39" t="s">
+      <c r="H40" s="24"/>
+      <c r="I40" s="23" t="s">
         <v>53</v>
       </c>
       <c r="J40" s="18">
@@ -2658,8 +2667,8 @@
         <f>S4</f>
         <v>-265.21739130434781</v>
       </c>
-      <c r="L40" s="40"/>
-      <c r="M40" s="45" t="s">
+      <c r="L40" s="24"/>
+      <c r="M40" s="29" t="s">
         <v>53</v>
       </c>
       <c r="N40" s="21">
@@ -2683,8 +2692,8 @@
         <f>K4</f>
         <v>448.5294117647058</v>
       </c>
-      <c r="D41" s="41"/>
-      <c r="E41" s="46" t="s">
+      <c r="D41" s="25"/>
+      <c r="E41" s="30" t="s">
         <v>54</v>
       </c>
       <c r="F41" s="21">
@@ -2693,8 +2702,8 @@
       <c r="G41" s="17">
         <v>376.33517495395944</v>
       </c>
-      <c r="H41" s="40"/>
-      <c r="I41" s="42" t="s">
+      <c r="H41" s="24"/>
+      <c r="I41" s="26" t="s">
         <v>43</v>
       </c>
       <c r="J41" s="18">
@@ -2705,8 +2714,8 @@
         <f>U4</f>
         <v>-1.4565217391304348</v>
       </c>
-      <c r="L41" s="40"/>
-      <c r="M41" s="46" t="s">
+      <c r="L41" s="24"/>
+      <c r="M41" s="30" t="s">
         <v>56</v>
       </c>
       <c r="N41" s="21">
@@ -2720,20 +2729,20 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
     </row>
     <row r="43" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="19" t="s">
@@ -2747,8 +2756,8 @@
         <f>I11</f>
         <v>157.35384615384615</v>
       </c>
-      <c r="D43" s="38"/>
-      <c r="E43" s="45" t="s">
+      <c r="D43" s="22"/>
+      <c r="E43" s="29" t="s">
         <v>42</v>
       </c>
       <c r="F43" s="21">
@@ -2758,8 +2767,8 @@
       <c r="G43" s="17">
         <v>721.73913043478262</v>
       </c>
-      <c r="H43" s="40"/>
-      <c r="I43" s="39" t="s">
+      <c r="H43" s="24"/>
+      <c r="I43" s="23" t="s">
         <v>52</v>
       </c>
       <c r="J43" s="18">
@@ -2770,8 +2779,8 @@
         <f>S11</f>
         <v>-100.82644628099173</v>
       </c>
-      <c r="L43" s="40"/>
-      <c r="M43" s="45" t="s">
+      <c r="L43" s="24"/>
+      <c r="M43" s="29" t="s">
         <v>52</v>
       </c>
       <c r="N43" s="21">
@@ -2795,8 +2804,8 @@
         <f>K11</f>
         <v>187.69230769230768</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="46" t="s">
+      <c r="D44" s="22"/>
+      <c r="E44" s="30" t="s">
         <v>55</v>
       </c>
       <c r="F44" s="21">
@@ -2805,8 +2814,8 @@
       <c r="G44" s="17">
         <v>-626.08695652173913</v>
       </c>
-      <c r="H44" s="40"/>
-      <c r="I44" s="42" t="s">
+      <c r="H44" s="24"/>
+      <c r="I44" s="26" t="s">
         <v>43</v>
       </c>
       <c r="J44" s="18">
@@ -2817,8 +2826,8 @@
         <f>U11</f>
         <v>-1.1900826446280992</v>
       </c>
-      <c r="L44" s="40"/>
-      <c r="M44" s="46" t="s">
+      <c r="L44" s="24"/>
+      <c r="M44" s="30" t="s">
         <v>57</v>
       </c>
       <c r="N44" s="21">
@@ -2832,20 +2841,20 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="40"/>
-      <c r="O45" s="40"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="24"/>
     </row>
     <row r="46" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="19" t="s">
@@ -2859,8 +2868,8 @@
         <f>I18</f>
         <v>605.88235294117646</v>
       </c>
-      <c r="D46" s="40"/>
-      <c r="E46" s="45" t="s">
+      <c r="D46" s="24"/>
+      <c r="E46" s="29" t="s">
         <v>45</v>
       </c>
       <c r="F46" s="21">
@@ -2871,8 +2880,8 @@
         <f>C40+C43</f>
         <v>467.6479638009049</v>
       </c>
-      <c r="H46" s="40"/>
-      <c r="I46" s="39" t="s">
+      <c r="H46" s="24"/>
+      <c r="I46" s="23" t="s">
         <v>48</v>
       </c>
       <c r="J46" s="18">
@@ -2883,8 +2892,8 @@
         <f>I28</f>
         <v>-515</v>
       </c>
-      <c r="L46" s="40"/>
-      <c r="M46" s="45" t="s">
+      <c r="L46" s="24"/>
+      <c r="M46" s="29" t="s">
         <v>48</v>
       </c>
       <c r="N46" s="21">
@@ -2907,8 +2916,8 @@
         <f>K11</f>
         <v>187.69230769230768</v>
       </c>
-      <c r="D47" s="40"/>
-      <c r="E47" s="47" t="s">
+      <c r="D47" s="24"/>
+      <c r="E47" s="31" t="s">
         <v>47</v>
       </c>
       <c r="F47" s="21">
@@ -2919,8 +2928,8 @@
         <f>C41+C44</f>
         <v>636.22171945701348</v>
       </c>
-      <c r="H47" s="40"/>
-      <c r="I47" s="42" t="s">
+      <c r="H47" s="24"/>
+      <c r="I47" s="26" t="s">
         <v>43</v>
       </c>
       <c r="J47" s="18">
@@ -2931,8 +2940,8 @@
         <f>K28</f>
         <v>-3.4166666666666665</v>
       </c>
-      <c r="L47" s="40"/>
-      <c r="M47" s="47" t="s">
+      <c r="L47" s="24"/>
+      <c r="M47" s="31" t="s">
         <v>47</v>
       </c>
       <c r="N47" s="21">
@@ -2944,20 +2953,20 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="48"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="44"/>
-      <c r="N48" s="40"/>
-      <c r="O48" s="40"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="24"/>
+      <c r="O48" s="24"/>
     </row>
     <row r="49" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
@@ -2971,8 +2980,8 @@
         <f>I23</f>
         <v>1.3430420711974112E-2</v>
       </c>
-      <c r="D49" s="40"/>
-      <c r="E49" s="45" t="s">
+      <c r="D49" s="24"/>
+      <c r="E49" s="29" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="21">
@@ -2983,8 +2992,8 @@
         <f>C37+G37</f>
         <v>1.7377049180327869E-2</v>
       </c>
-      <c r="H49" s="40"/>
-      <c r="I49" s="39" t="s">
+      <c r="H49" s="24"/>
+      <c r="I49" s="23" t="s">
         <v>49</v>
       </c>
       <c r="J49" s="18">
@@ -2995,8 +3004,8 @@
         <f>I33</f>
         <v>-468.18181818181813</v>
       </c>
-      <c r="L49" s="40"/>
-      <c r="M49" s="45" t="s">
+      <c r="L49" s="24"/>
+      <c r="M49" s="29" t="s">
         <v>49</v>
       </c>
       <c r="N49" s="21">
@@ -3019,8 +3028,8 @@
         <f>K23</f>
         <v>1.8608414239482201E-3</v>
       </c>
-      <c r="D50" s="40"/>
-      <c r="E50" s="47" t="s">
+      <c r="D50" s="24"/>
+      <c r="E50" s="31" t="s">
         <v>47</v>
       </c>
       <c r="F50" s="21">
@@ -3031,8 +3040,8 @@
         <f>C38+G38</f>
         <v>1.5081967213114757E-2</v>
       </c>
-      <c r="H50" s="40"/>
-      <c r="I50" s="42" t="s">
+      <c r="H50" s="24"/>
+      <c r="I50" s="26" t="s">
         <v>43</v>
       </c>
       <c r="J50" s="18">
@@ -3043,8 +3052,8 @@
         <f>K33</f>
         <v>-2.1969696969696968</v>
       </c>
-      <c r="L50" s="40"/>
-      <c r="M50" s="47" t="s">
+      <c r="L50" s="24"/>
+      <c r="M50" s="31" t="s">
         <v>47</v>
       </c>
       <c r="N50" s="21">
@@ -3056,26 +3065,42 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="44"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="40"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M17:P24">
     <sortCondition ref="O17:O24"/>
   </sortState>
   <mergeCells count="31">
+    <mergeCell ref="A35:O35"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="H31:K31"/>
     <mergeCell ref="H25:K25"/>
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="R1:U1"/>
@@ -3091,22 +3116,6 @@
     <mergeCell ref="N20:P20"/>
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="N15:P15"/>
-    <mergeCell ref="A35:N35"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="H31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3124,21 +3133,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="G1" s="35" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
+      <c r="G1" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
delirio místico de signos
</commit_message>
<xml_diff>
--- a/TP5/Mediciones.xlsx
+++ b/TP5/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\source\repos\TP3-Electro\TP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3737CB4A-96D3-4841-ADE2-8F00DFC19311}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7491D6C-B81E-4C2E-911D-D7192B3CFC81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FDA36349-2CEE-46F1-A8FD-45D31E04EF72}"/>
   </bookViews>
@@ -1058,6 +1058,42 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1110,42 +1146,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1234583-11C2-4965-B267-EB43A84ACFA3}">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,32 +1482,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
-      <c r="H1" s="46" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="66"/>
+      <c r="H1" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="63" t="s">
+      <c r="M1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="R1" s="60" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="R1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -1523,28 +1523,28 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="58" t="str">
+      <c r="H2" s="42" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="58" t="str">
+      <c r="M2" s="42" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="R2" s="58" t="str">
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="R2" s="42" t="str">
         <f>$A$1</f>
         <v>Cuadripolo "B" - Nro. De serie: 9608 (15 V - 50 mA) (T)</v>
       </c>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
     </row>
     <row r="3" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -1775,34 +1775,34 @@
       <c r="W7" s="33"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="M8" s="65" t="s">
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="M8" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
       <c r="Q8" s="24"/>
-      <c r="R8" s="61" t="s">
+      <c r="R8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="S8" s="61"/>
-      <c r="T8" s="61"/>
-      <c r="U8" s="61"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
       <c r="W8" s="33"/>
     </row>
     <row r="9" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -1821,28 +1821,28 @@
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
-      <c r="H9" s="47" t="str">
+      <c r="H9" s="59" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="M9" s="62" t="str">
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="M9" s="44" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
       <c r="Q9" s="24"/>
-      <c r="R9" s="62" t="str">
+      <c r="R9" s="44" t="str">
         <f>$A$8</f>
         <v>Cuadripolo "A" - Nro. De serie: 9603 (15 V - 50 mA) (Pi)</v>
       </c>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
       <c r="W9" s="33"/>
     </row>
     <row r="10" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -1964,20 +1964,20 @@
         <v>6.3549704947798462</v>
       </c>
       <c r="S11" s="7">
-        <f>B11/E11*1000</f>
-        <v>100.82644628099173</v>
+        <f>-B11/E11*1000</f>
+        <v>-100.82644628099173</v>
       </c>
       <c r="T11" s="7">
         <f>D13/C13/1000</f>
         <v>6.3549704947798462E-3</v>
       </c>
       <c r="U11" s="7">
-        <f>D11/E11</f>
-        <v>1.1900826446280992</v>
+        <f>-D11/E11</f>
+        <v>-1.1900826446280992</v>
       </c>
       <c r="W11" s="13">
         <f>R11*U11-S11*T11</f>
-        <v>6.9221910017519317</v>
+        <v>-6.9221910017519317</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -2045,26 +2045,26 @@
       <c r="K14" s="33"/>
     </row>
     <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="33"/>
       <c r="G15" s="33"/>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="50"/>
-      <c r="N15" s="69" t="s">
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
+      <c r="N15" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
     </row>
     <row r="16" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="36"/>
@@ -2082,17 +2082,17 @@
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
-      <c r="H16" s="43" t="s">
+      <c r="H16" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="45"/>
-      <c r="N16" s="66" t="s">
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
+      <c r="N16" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="67"/>
-      <c r="P16" s="68"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="50"/>
     </row>
     <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
@@ -2126,11 +2126,11 @@
       <c r="K17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="N17" s="66" t="s">
+      <c r="N17" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="67"/>
-      <c r="P17" s="68"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="50"/>
     </row>
     <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
@@ -2183,26 +2183,26 @@
       <c r="K19" s="33"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="45"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="33"/>
       <c r="G20" s="33"/>
-      <c r="H20" s="51" t="s">
+      <c r="H20" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="N20" s="66" t="s">
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="N20" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="O20" s="67"/>
-      <c r="P20" s="68"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="50"/>
     </row>
     <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="36"/>
@@ -2220,12 +2220,12 @@
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
-      <c r="H21" s="47" t="s">
+      <c r="H21" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
@@ -2311,21 +2311,21 @@
       <c r="K24" s="33"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
-      <c r="H25" s="59" t="s">
+      <c r="H25" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
     </row>
     <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="36"/>
@@ -2343,12 +2343,12 @@
       </c>
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
-      <c r="H26" s="47" t="s">
+      <c r="H26" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2411,20 +2411,20 @@
         <v>2.2888888888888888</v>
       </c>
       <c r="I28" s="13">
-        <f>B27/E27*1000</f>
-        <v>515</v>
+        <f>-B27/E27*1000</f>
+        <v>-515</v>
       </c>
       <c r="J28" s="13">
         <f>D28/C28/1000</f>
         <v>1.3148148148148147E-2</v>
       </c>
       <c r="K28" s="13">
-        <f>D27/E27</f>
-        <v>3.4166666666666665</v>
+        <f>-D27/E27</f>
+        <v>-3.4166666666666665</v>
       </c>
       <c r="M28" s="13">
         <f>H28*K28-I28*J28</f>
-        <v>1.049074074074074</v>
+        <v>-1.049074074074074</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2442,21 +2442,21 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
-      <c r="H30" s="59" t="s">
+      <c r="H30" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="59"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
       <c r="M30" s="12"/>
     </row>
     <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2475,12 +2475,12 @@
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
-      <c r="H31" s="47" t="s">
+      <c r="H31" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
       <c r="M31" s="12"/>
     </row>
     <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
@@ -2543,40 +2543,40 @@
         <v>3.5558112773302644</v>
       </c>
       <c r="I33" s="13">
-        <f>B32/E32*1000</f>
-        <v>468.18181818181813</v>
+        <f>-B32/E32*1000</f>
+        <v>-468.18181818181813</v>
       </c>
       <c r="J33" s="13">
         <f>E32/B33/1000</f>
         <v>2.1359223300970879E-3</v>
       </c>
       <c r="K33" s="13">
-        <f>D32/E32</f>
-        <v>2.1969696969696968</v>
+        <f>-D32/E32</f>
+        <v>-2.1969696969696968</v>
       </c>
       <c r="M33" s="13">
         <f>H33*K33-I33*J33</f>
-        <v>6.8120096244377013</v>
+        <v>-6.8120096244377013</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41"/>
-      <c r="M35" s="41"/>
-      <c r="N35" s="41"/>
-      <c r="O35" s="42"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="54"/>
     </row>
     <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="19" t="s">
@@ -2806,7 +2806,7 @@
       </c>
       <c r="K43" s="14">
         <f>S11</f>
-        <v>100.82644628099173</v>
+        <v>-100.82644628099173</v>
       </c>
       <c r="L43" s="24"/>
       <c r="M43" s="29" t="s">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="K44" s="14">
         <f>U11</f>
-        <v>1.1900826446280992</v>
+        <v>-1.1900826446280992</v>
       </c>
       <c r="L44" s="24"/>
       <c r="M44" s="30" t="s">
@@ -2919,7 +2919,7 @@
       </c>
       <c r="K46" s="14">
         <f>I28</f>
-        <v>515</v>
+        <v>-515</v>
       </c>
       <c r="L46" s="24"/>
       <c r="M46" s="29" t="s">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="K47" s="14">
         <f>K28</f>
-        <v>3.4166666666666665</v>
+        <v>-3.4166666666666665</v>
       </c>
       <c r="L47" s="24"/>
       <c r="M47" s="31" t="s">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="K49" s="14">
         <f>I33</f>
-        <v>468.18181818181813</v>
+        <v>-468.18181818181813</v>
       </c>
       <c r="L49" s="24"/>
       <c r="M49" s="29" t="s">
@@ -3079,7 +3079,7 @@
       </c>
       <c r="K50" s="14">
         <f>K33</f>
-        <v>2.1969696969696968</v>
+        <v>-2.1969696969696968</v>
       </c>
       <c r="L50" s="24"/>
       <c r="M50" s="31" t="s">
@@ -3114,21 +3114,6 @@
     <sortCondition ref="O17:O24"/>
   </sortState>
   <mergeCells count="31">
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N15:P15"/>
     <mergeCell ref="A35:O35"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H1:K1"/>
@@ -3145,6 +3130,21 @@
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="N15:P15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3162,13 +3162,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="66"/>
       <c r="G1" s="70" t="s">
         <v>28</v>
       </c>

</xml_diff>